<commit_message>
sửa ít nhỏ nhỏ
</commit_message>
<xml_diff>
--- a/upload/file_mau/bang_tong_hop_danh_gia_ren_luyen.xlsx
+++ b/upload/file_mau/bang_tong_hop_danh_gia_ren_luyen.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Laravel\luanvantotnghiep\public\upload\file_mau\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Laravel\luanvantotnghiep\upload\file_mau\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -913,23 +913,23 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1915,7 +1915,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -2038,17 +2038,17 @@
     <row r="8" spans="1:15" s="26" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="29"/>
       <c r="C8" s="5"/>
-      <c r="E8" s="75" t="s">
+      <c r="E8" s="78" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="75"/>
-      <c r="G8" s="75"/>
-      <c r="H8" s="75"/>
-      <c r="I8" s="75"/>
-      <c r="J8" s="75"/>
-      <c r="K8" s="75"/>
-      <c r="L8" s="75"/>
-      <c r="M8" s="75"/>
+      <c r="F8" s="78"/>
+      <c r="G8" s="78"/>
+      <c r="H8" s="78"/>
+      <c r="I8" s="78"/>
+      <c r="J8" s="78"/>
+      <c r="K8" s="78"/>
+      <c r="L8" s="78"/>
+      <c r="M8" s="78"/>
     </row>
     <row r="9" spans="1:15" s="26" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="29"/>
@@ -2065,7 +2065,7 @@
       <c r="L9" s="72"/>
       <c r="M9" s="72"/>
     </row>
-    <row r="10" spans="1:15" s="26" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" s="26" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="29"/>
     </row>
     <row r="11" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
@@ -2075,37 +2075,37 @@
       <c r="B11" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="76" t="s">
+      <c r="C11" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="76"/>
+      <c r="D11" s="77"/>
       <c r="E11" s="83" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="76" t="s">
+      <c r="F11" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="76"/>
-      <c r="H11" s="76"/>
-      <c r="I11" s="76" t="s">
+      <c r="G11" s="77"/>
+      <c r="H11" s="77"/>
+      <c r="I11" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="J11" s="76" t="s">
+      <c r="J11" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="K11" s="76" t="s">
+      <c r="K11" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="L11" s="76" t="s">
+      <c r="L11" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="M11" s="76" t="s">
+      <c r="M11" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="N11" s="76" t="s">
+      <c r="N11" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="O11" s="77" t="s">
+      <c r="O11" s="79" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2130,7 +2130,7 @@
       <c r="L12" s="59"/>
       <c r="M12" s="59"/>
       <c r="N12" s="59"/>
-      <c r="O12" s="78"/>
+      <c r="O12" s="80"/>
     </row>
     <row r="13" spans="1:15" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="51" t="s">
@@ -2139,10 +2139,10 @@
       <c r="B13" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="79" t="s">
+      <c r="C13" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="80"/>
+      <c r="D13" s="76"/>
       <c r="E13" s="53" t="s">
         <v>21</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="23.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A14" s="44"/>
       <c r="B14" s="45"/>
       <c r="C14" s="46"/>
@@ -2194,7 +2194,7 @@
       <c r="N14" s="49"/>
       <c r="O14" s="50"/>
     </row>
-    <row r="15" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="35"/>
       <c r="B15" s="11"/>
       <c r="C15" s="12"/>
@@ -2211,7 +2211,7 @@
       <c r="N15" s="15"/>
       <c r="O15" s="36"/>
     </row>
-    <row r="16" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="35"/>
       <c r="B16" s="14"/>
       <c r="C16" s="12"/>
@@ -2228,7 +2228,7 @@
       <c r="N16" s="15"/>
       <c r="O16" s="36"/>
     </row>
-    <row r="17" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="35"/>
       <c r="B17" s="14"/>
       <c r="C17" s="12"/>
@@ -2245,7 +2245,7 @@
       <c r="N17" s="15"/>
       <c r="O17" s="36"/>
     </row>
-    <row r="18" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="35"/>
       <c r="B18" s="11"/>
       <c r="C18" s="12"/>
@@ -2262,7 +2262,7 @@
       <c r="N18" s="15"/>
       <c r="O18" s="36"/>
     </row>
-    <row r="19" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="35"/>
       <c r="B19" s="11"/>
       <c r="C19" s="12"/>
@@ -2279,7 +2279,7 @@
       <c r="N19" s="15"/>
       <c r="O19" s="36"/>
     </row>
-    <row r="20" spans="1:15" s="30" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="35"/>
       <c r="B20" s="11"/>
       <c r="C20" s="12"/>
@@ -2296,7 +2296,7 @@
       <c r="N20" s="15"/>
       <c r="O20" s="36"/>
     </row>
-    <row r="21" spans="1:15" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="37"/>
       <c r="B21" s="38"/>
       <c r="C21" s="39"/>

</xml_diff>